<commit_message>
update ref and minor correction
</commit_message>
<xml_diff>
--- a/rw_vaccine_details.xlsx
+++ b/rw_vaccine_details.xlsx
@@ -5692,7 +5692,7 @@
       </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+          <t>ToledoRomani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
         </is>
       </c>
       <c r="Y52" t="inlineStr"/>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+          <t>ToledoRomani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
         </is>
       </c>
       <c r="Y53" t="n">
@@ -5898,7 +5898,7 @@
       </c>
       <c r="X54" t="inlineStr">
         <is>
-          <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+          <t>ToledoRomani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
         </is>
       </c>
       <c r="Y54" t="inlineStr"/>
@@ -5996,7 +5996,7 @@
       </c>
       <c r="X55" t="inlineStr">
         <is>
-          <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+          <t>ToledoRomani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
         </is>
       </c>
       <c r="Y55" t="inlineStr"/>
@@ -6098,7 +6098,7 @@
       </c>
       <c r="X56" t="inlineStr">
         <is>
-          <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+          <t>ToledoRomani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
         </is>
       </c>
       <c r="Y56" t="inlineStr"/>
@@ -6200,7 +6200,7 @@
       </c>
       <c r="X57" t="inlineStr">
         <is>
-          <t>Romani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
+          <t>ToledoRomani2021_Efficacy_and_safety_SOBERANA_02_a_COVID-19</t>
         </is>
       </c>
       <c r="Y57" t="inlineStr"/>
@@ -6704,7 +6704,7 @@
       </c>
       <c r="X62" t="inlineStr">
         <is>
-          <t>Sahly2021_efficacy_of_the_mRNA-1273_SARS_C0V-2_vaccine</t>
+          <t>El2021_efficacy_of_the_mRNA-1273_SARS_C0V-2_vaccine</t>
         </is>
       </c>
       <c r="Y62" t="inlineStr"/>
@@ -6804,7 +6804,7 @@
       </c>
       <c r="X63" t="inlineStr">
         <is>
-          <t>Sahly2021_efficacy_of_the_mRNA-1273_SARS_C0V-2_vaccine</t>
+          <t>El2021_efficacy_of_the_mRNA-1273_SARS_C0V-2_vaccine</t>
         </is>
       </c>
       <c r="Y63" t="inlineStr"/>

</xml_diff>

<commit_message>
add PythonMeta test code
</commit_message>
<xml_diff>
--- a/rw_vaccine_details.xlsx
+++ b/rw_vaccine_details.xlsx
@@ -1657,13 +1657,13 @@
       </c>
       <c r="Y12" t="inlineStr"/>
       <c r="Z12" t="n">
-        <v>100</v>
+        <v>94.43796319779074</v>
       </c>
       <c r="AA12" t="n">
-        <v>0</v>
+        <v>-3.302327052537257</v>
       </c>
       <c r="AB12" t="n">
-        <v>0</v>
+        <v>99.70052704259608</v>
       </c>
     </row>
     <row r="13">
@@ -2761,13 +2761,13 @@
       </c>
       <c r="Y23" t="inlineStr"/>
       <c r="Z23" t="n">
-        <v>100</v>
+        <v>97.15223914397328</v>
       </c>
       <c r="AA23" t="n">
-        <v>0</v>
+        <v>50.66493499150665</v>
       </c>
       <c r="AB23" t="n">
-        <v>0</v>
+        <v>99.83561911002404</v>
       </c>
     </row>
     <row r="24">
@@ -3061,13 +3061,13 @@
       </c>
       <c r="Y26" t="inlineStr"/>
       <c r="Z26" t="n">
-        <v>100</v>
+        <v>83.86268848251524</v>
       </c>
       <c r="AA26" t="n">
-        <v>0</v>
+        <v>-296.1118075190292</v>
       </c>
       <c r="AB26" t="n">
-        <v>0</v>
+        <v>99.34257747921377</v>
       </c>
     </row>
     <row r="27">
@@ -3161,13 +3161,13 @@
       </c>
       <c r="Y27" t="inlineStr"/>
       <c r="Z27" t="n">
-        <v>100</v>
+        <v>96.97505086197665</v>
       </c>
       <c r="AA27" t="n">
-        <v>0</v>
+        <v>49.63835990348066</v>
       </c>
       <c r="AB27" t="n">
-        <v>0</v>
+        <v>99.8183077979571</v>
       </c>
     </row>
     <row r="28">
@@ -3463,13 +3463,13 @@
       </c>
       <c r="Y30" t="inlineStr"/>
       <c r="Z30" t="n">
-        <v>100</v>
+        <v>85.72256728778468</v>
       </c>
       <c r="AA30" t="n">
-        <v>0</v>
+        <v>-176.3903643897301</v>
       </c>
       <c r="AB30" t="n">
-        <v>0</v>
+        <v>99.2624739820365</v>
       </c>
     </row>
     <row r="31">
@@ -4073,13 +4073,13 @@
       </c>
       <c r="Y36" t="inlineStr"/>
       <c r="Z36" t="n">
-        <v>100</v>
+        <v>94.5169636319258</v>
       </c>
       <c r="AA36" t="n">
-        <v>0</v>
+        <v>5.021905453613229</v>
       </c>
       <c r="AB36" t="n">
-        <v>0</v>
+        <v>99.68346714095279</v>
       </c>
     </row>
     <row r="37">
@@ -5095,13 +5095,13 @@
       </c>
       <c r="Y46" t="inlineStr"/>
       <c r="Z46" t="n">
-        <v>100</v>
+        <v>99.2008996601827</v>
       </c>
       <c r="AA46" t="n">
-        <v>0</v>
+        <v>86.7896061036983</v>
       </c>
       <c r="AB46" t="n">
-        <v>0</v>
+        <v>99.95166220189128</v>
       </c>
     </row>
     <row r="47">
@@ -5397,13 +5397,13 @@
       </c>
       <c r="Y49" t="inlineStr"/>
       <c r="Z49" t="n">
-        <v>100</v>
+        <v>95.31787684795356</v>
       </c>
       <c r="AA49" t="n">
-        <v>0</v>
+        <v>20.11694832456909</v>
       </c>
       <c r="AB49" t="n">
-        <v>0</v>
+        <v>99.72557035877897</v>
       </c>
     </row>
     <row r="50">
@@ -5499,13 +5499,13 @@
       </c>
       <c r="Y50" t="inlineStr"/>
       <c r="Z50" t="n">
-        <v>100</v>
+        <v>92.43657029284805</v>
       </c>
       <c r="AA50" t="n">
-        <v>0</v>
+        <v>-34.22888656146353</v>
       </c>
       <c r="AB50" t="n">
-        <v>0</v>
+        <v>99.57382147464335</v>
       </c>
     </row>
     <row r="51">
@@ -6103,13 +6103,13 @@
       </c>
       <c r="Y56" t="inlineStr"/>
       <c r="Z56" t="n">
-        <v>100</v>
+        <v>92.07499501362942</v>
       </c>
       <c r="AA56" t="n">
-        <v>0</v>
+        <v>-40.6707088182735</v>
       </c>
       <c r="AB56" t="n">
-        <v>0</v>
+        <v>99.5535267820742</v>
       </c>
     </row>
     <row r="57">
@@ -6205,13 +6205,13 @@
       </c>
       <c r="Y57" t="inlineStr"/>
       <c r="Z57" t="n">
-        <v>100</v>
+        <v>93.93970206924602</v>
       </c>
       <c r="AA57" t="n">
-        <v>0</v>
+        <v>-4.991807763674427</v>
       </c>
       <c r="AB57" t="n">
-        <v>0</v>
+        <v>99.65018974535451</v>
       </c>
     </row>
     <row r="58">

</xml_diff>